<commit_message>
update README and add screenshots
</commit_message>
<xml_diff>
--- a/xls/crews_cb_3.xlsx
+++ b/xls/crews_cb_3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\UCB2204\home\cb\projects\dev\crewAI-xls\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B66A07BF-2B4B-4481-B60E-955A92A75026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9B9CDA6-CFB4-4638-99A7-651BEE58E210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2414,7 +2414,7 @@
   <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="A9" sqref="A9:N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2934,8 +2934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2952,13 +2952,13 @@
     <col min="10" max="10" width="11.42578125" style="1" customWidth="1"/>
     <col min="11" max="11" width="10.28515625" style="1" customWidth="1"/>
     <col min="12" max="12" width="18.5703125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="15" style="1" customWidth="1"/>
-    <col min="14" max="17" width="10.5703125" style="1" customWidth="1"/>
+    <col min="13" max="14" width="15" style="1" customWidth="1"/>
+    <col min="15" max="17" width="10.5703125" style="1" customWidth="1"/>
     <col min="18" max="18" width="11" style="1" customWidth="1"/>
     <col min="19" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="45">
+    <row r="1" spans="1:18" ht="30">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -3220,7 +3220,7 @@
         <v>376</v>
       </c>
       <c r="I8" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J8" s="1">
         <v>30</v>
@@ -3264,7 +3264,7 @@
         <v>376</v>
       </c>
       <c r="I9" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J9" s="1">
         <v>30</v>
@@ -3422,7 +3422,10 @@
   <dimension ref="A1:U21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>